<commit_message>
Arquivo para consulta no termional
</commit_message>
<xml_diff>
--- a/Especies.xlsx
+++ b/Especies.xlsx
@@ -2224,6 +2224,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:M86" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
+  <autoFilter ref="A2:M86"/>
+  <tableColumns count="13">
+    <tableColumn name="Item" id="1" totalsRowLabel="Total"/>
+    <tableColumn name="Espécie" id="2"/>
+    <tableColumn name="Categoria de risco de extinção " id="3"/>
+    <tableColumn name="Critérios" id="4"/>
+    <tableColumn name="Bacia" id="5"/>
+    <tableColumn name="Localização" id="6"/>
+    <tableColumn name="Obs. Localidade" id="7"/>
+    <tableColumn name="Ameaça (resumida)" id="8"/>
+    <tableColumn name="Obs. Ameaça" id="9"/>
+    <tableColumn name="PAN" id="10"/>
+    <tableColumn name="Presença em UC" id="11"/>
+    <tableColumn name="Pesquisas" id="12"/>
+    <tableColumn name="Ações" id="13" totalsRowFunction="custom">
+      <totalsRowFormula>Sum</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5624,5 +5648,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A api já funciona e tem alguns filtros
</commit_message>
<xml_diff>
--- a/Especies.xlsx
+++ b/Especies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="466">
   <si>
     <t>Item</t>
   </si>
@@ -2016,7 +2016,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2026,13 +2026,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFff0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2060,7 +2066,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2137,11 +2143,18 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2194,11 +2207,20 @@
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2246,7 +2268,7 @@
       <totalsRowFormula>Sum</totalsRowFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -2538,7 +2560,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
@@ -2546,19 +2568,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="20" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="21" width="47.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="21" width="52.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="21" width="52.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="22" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="23" width="26.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="23" width="68.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="22" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="23" width="82.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="22" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="22" width="34.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="22" width="49.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="22" width="66.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="23" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="24" width="47.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="24" width="52.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="24" width="52.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="25" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="26" width="26.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="26" width="68.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="25" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="26" width="82.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="25" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="25" width="34.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="25" width="49.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="25" width="66.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
@@ -2633,11 +2655,15 @@
       <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="7"/>
+      <c r="M2" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="37.5">
       <c r="A3" s="8">
@@ -3766,7 +3792,7 @@
         <v>227</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="207.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="147">
       <c r="A32" s="1" t="s">
         <v>228</v>
       </c>
@@ -3805,7 +3831,7 @@
         <v>233</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="138">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="108.75">
       <c r="A33" s="1" t="s">
         <v>234</v>
       </c>
@@ -5646,6 +5672,21 @@
       <c r="L85" s="7"/>
       <c r="M85" s="7"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="16.5">
+      <c r="A86" s="20"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="19"/>
+      <c r="J86" s="22"/>
+      <c r="K86" s="22"/>
+      <c r="L86" s="22"/>
+      <c r="M86" s="22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>